<commit_message>
Entregas 1, 2 y 3
</commit_message>
<xml_diff>
--- a/inge-informes/Entrega 5/Test Cases.xlsx
+++ b/inge-informes/Entrega 5/Test Cases.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="89">
   <si>
     <t>CASO DE USO :</t>
   </si>
@@ -56,7 +56,7 @@
       <t xml:space="preserve">Registro </t>
     </r>
     <r>
-      <t>- Un registrario registra con un mail nueva, los campos completados y una contraseña correcta.</t>
+      <t>- Un registrario registra con un mail nuevo en formato correcto y una contraseña correcta.</t>
     </r>
   </si>
   <si>
@@ -86,7 +86,7 @@
       <rPr>
         <rFont val="Calibri"/>
       </rPr>
-      <t>- Un registrario registra con un mail ya registrado, los campos completados o una contraseña incorrecta.</t>
+      <t>- Un registrario registra con un mail ya registrado y una contraseña incorrecta.</t>
     </r>
   </si>
   <si>
@@ -96,13 +96,49 @@
     <t>El usuario no puede tener acceso al sistema como si la registración había sido exitosa.</t>
   </si>
   <si>
-    <t>EL sistema debe que mostrar un mensaje de error.</t>
+    <t xml:space="preserve">El sistema debe mostrar un mensaje de error diciendo que el mail ya está registrado y que la contraseña debe seguir las directrises. </t>
   </si>
   <si>
     <t>El sistema tiene que volver el usuario a la pantalla de registro.</t>
   </si>
   <si>
     <t xml:space="preserve"> El sistema muestra un mensaje de error, solicita al usuario ingresar nuevamente los datos, mostrando el error. Vuelve a la pantalla del registro.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+      </rPr>
+      <t xml:space="preserve">Registro </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>- Un registrario registra con un mail ya registrado, pero con una contraseña correcta.</t>
+    </r>
+  </si>
+  <si>
+    <t>El sistema debe mostrar un mensaje de error diciendo que el mail ya está registrado.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+      </rPr>
+      <t xml:space="preserve">Registro </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>- Un registrario registra con un mail nuevo en formato correcto, pero con una contraseña incorrecta.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">El sistema debe mostrar un mensaje de error diciendo que el formato de la contraseña debe seguir las directrises. </t>
   </si>
   <si>
     <t>CU2</t>
@@ -113,7 +149,7 @@
     </r>
     <r>
       <rPr/>
-      <t xml:space="preserve"> - El usuario empieza en la pantalla de login e ingresa sus datos correctamente.</t>
+      <t xml:space="preserve"> - El usuario empieza en la pantalla de login e ingresa su nombre de usuario y su contraseña correctamente.</t>
     </r>
   </si>
   <si>
@@ -121,15 +157,15 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Login - </t>
+      <t>Login</t>
     </r>
     <r>
       <rPr/>
-      <t>El usuario empieza en la pantalla de login y ingresa sus datos incorrectamente.</t>
+      <t xml:space="preserve"> - El usuario empieza en la pantalla de login e ingresa su nombre de usuario correctamente pero su contraseña incorrectamente.</t>
     </r>
   </si>
   <si>
-    <t>El sistema solicita al usuario ingresar nuevamente los datos, mostrando el error.</t>
+    <t>El sistema solicita al usuario ingresar nuevamente la contraseña.</t>
   </si>
   <si>
     <t>El usuario no puede tener acceso al sistema como si el login había sido exitosa.</t>
@@ -138,7 +174,7 @@
     <t>El sistema tiene que volver el usuario a la pantalla de login.</t>
   </si>
   <si>
-    <t>El sistema vuelve el usuario a la plantalla de login. El login no ha sido exitoso</t>
+    <t>El sistema borra la contraseña y pide la usuario a ingresarla de nuevo. El login no ha sido exitoso</t>
   </si>
   <si>
     <r>
@@ -167,7 +203,7 @@
     </r>
     <r>
       <rPr/>
-      <t>El usuario empieza en la pantalla de incicio del restaurante y selecciona los platos con éxito. El restaurante confirma el pedido.</t>
+      <t>El usuario empieza en la pantalla de incicio del restaurante y selecciona los platos que desea. El restaurante confirma el pedido.</t>
     </r>
   </si>
   <si>
@@ -188,7 +224,7 @@
     </r>
     <r>
       <rPr/>
-      <t>El usuario empieza en la pantalla de incicio del restaurante y selecciona los platos con éxito. El restaurante rechaza el pedido.</t>
+      <t>El usuario empieza en la pantalla de incicio del restaurante y selecciona los platos que desea. El restaurante rechaza el pedido.</t>
     </r>
   </si>
   <si>
@@ -212,7 +248,7 @@
     </r>
     <r>
       <rPr/>
-      <t>Un administrador del restaurante toca el botón "Modificar datos", modifica los datos, toca el botón "Guardar cambios" y el sistema realiza los cambios.</t>
+      <t>Un administrador del restaurante toca el botón "Modificar datos", modifica los datos (nombre, ubicación), toca el botón "Guardar cambios" y el sistema realiza los cambios.</t>
     </r>
   </si>
   <si>
@@ -230,7 +266,7 @@
     </r>
     <r>
       <rPr/>
-      <t>Un administrador del restaurante selecciona un producto del menu, toca el botón "Modificar el producto", realiza los cambios que desee con datos válidos, toca el botón "Guardar cambios" y el sistema realiza los cambios.</t>
+      <t>Un administrador del restaurante selecciona un producto del menu, toca el botón "Modificar el producto", realiza los cambios que desee manteniendo el precio mayor de 0 ARS después de los cambios, toca el botón "Guardar cambios" y el sistema realiza los cambios.</t>
     </r>
   </si>
   <si>
@@ -239,14 +275,14 @@
     </r>
     <r>
       <rPr/>
-      <t>Un administrador del restaurante selecciona un producto del menu, toca el botón "Modificar el producto", realiza los cambios que desee con datos inválidos, toca el botón "Guardar cambios" y el sistema realiza los cambios.</t>
+      <t>Un administrador del restaurante selecciona un producto del menu, toca el botón "Modificar el producto", realiza los cambios que desee pero ingresa un precio menor de 0 ARS, toca el botón "Guardar cambios".</t>
     </r>
   </si>
   <si>
     <t>Los cambios no son realizados</t>
   </si>
   <si>
-    <t>Un mensaje de error se muestran en la pantalla.</t>
+    <t>Un mensaje de error se muestran en la pantalla diciendo que el precio tiene que ser mayor de 0 ARS.</t>
   </si>
   <si>
     <t>El administrador vuelve al producto.</t>
@@ -263,7 +299,7 @@
     </r>
     <r>
       <rPr/>
-      <t>El usuario abri el tab del perfil. El sistema muestra los datos del usuario, con opción a editar. El usuario cambiarlos con datos válidos, toca el botón "Guardar cambios" y el sistema guarda los nuevos datos y envía el usuario a la pantalla del perfil.</t>
+      <t>El usuario abri el tab del perfil. El sistema muestra los datos del usuario (nombre, apellido, email, contraseña), con opción a editar. El usuario cambiarlos con un mail en formato correcto y una contraseña correcta, toca el botón "Guardar cambios" y el sistema guarda los nuevos datos y envía el usuario a la pantalla del perfil.</t>
     </r>
   </si>
   <si>
@@ -278,11 +314,38 @@
     </r>
     <r>
       <rPr/>
-      <t>El usuario abri el tab del perfil. El sistema muestra los datos del usuario, con opción a editar. El usuario cambiarlos con datos inválidos, toca el botón "Guardar cambios" y el sistema guarda los nuevos datos y envía el usuario a la pantalla del perfil.</t>
+      <t>El usuario abri el tab del perfil. El sistema muestra los datos del usuario, con opción a editar. El usuario cambiarlos con un mail en formato correcto pero con una contraseña incorrecta, toca el botón "Guardar cambios" y el sistema guarda los nuevos datos y envía el usuario a la pantalla del perfil.</t>
     </r>
   </si>
   <si>
+    <t xml:space="preserve">El sistema debe mostrar un mensaje de error diciendo que  la contraseña debe seguir las directrises. </t>
+  </si>
+  <si>
     <t>Los cambios no son realizados. El usuario vuelve al perfil.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Modificación de los datos de usuario - </t>
+    </r>
+    <r>
+      <rPr/>
+      <t>El usuario abri el tab del perfil. El sistema muestra los datos del usuario, con opción a editar. El usuario cambiarlos con un mail en formato incorrecto pero con una contraseña correcta, toca el botón "Guardar cambios" y el sistema guarda los nuevos datos y envía el usuario a la pantalla del perfil.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">El sistema debe mostrar un mensaje de error diciendo que  el email debe seguir las directrises. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Modificación de los datos de usuario - </t>
+    </r>
+    <r>
+      <rPr/>
+      <t>El usuario abri el tab del perfil. El sistema muestra los datos del usuario, con opción a editar. El usuario cambiarlos con un mail en formato incorrecto, una contraseña incorrecta, toca el botón "Guardar cambios" y el sistema guarda los nuevos datos y envía el usuario a la pantalla del perfil.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">El sistema debe mostrar un mensaje de error diciendo que el nuevo email y la contraseña debe seguir las directrises. </t>
   </si>
   <si>
     <t>CU10</t>
@@ -348,7 +411,7 @@
       <t xml:space="preserve">Alta de Producto - . </t>
     </r>
     <r>
-      <t xml:space="preserve">El administrador se dirige a menú y selecciona en el botón “+” (agregar producto). El sistema muestra la pantalla de agregar producto,  después de lo cual el administrador ingresa datos válidos del producto. El sistema verifica que todos los datos sean ingresados con datos válidos, añade el producto a la base de datos,  muestra un mensaje de éxito y envia el administrador a la pantalla de inicio
+      <t xml:space="preserve">El administrador se dirige a menú y selecciona en el botón “+” (agregar producto). El sistema muestra la pantalla de agregar producto,  después de lo cual el administrador ingresa datos válidos del producto. El sistema verifica que el precio sea mayor de 0 ARS, añade el producto a la base de datos,  muestra un mensaje de éxito y envia el administrador a la pantalla de inicio
 </t>
     </r>
   </si>
@@ -366,15 +429,12 @@
       <rPr>
         <b/>
       </rPr>
-      <t xml:space="preserve">Alta de Producto - . </t>
+      <t xml:space="preserve">Alta de Producto - </t>
     </r>
     <r>
-      <t xml:space="preserve">El administrador se dirige a menú y selecciona en el botón “+” (agregar producto). El sistema muestra la pantalla de agregar producto,  después de lo cual el administrador ingresa datos inválidos del producto. Un mensaje de error se muestra y el administrador vuelve a la pantalla de inicio.
+      <t xml:space="preserve">El administrador se dirige a menú y selecciona en el botón “+” (agregar producto). El sistema muestra la pantalla de agregar producto,  después de lo cual el administrador ingresa un precio menor de 0 ARS. Un mensaje de error se muestra y el administrador vuelve a la pantalla de inicio.
 </t>
     </r>
-  </si>
-  <si>
-    <t>Un mensaje de error se muestra en la pantalla.</t>
   </si>
   <si>
     <t>Los cambios no son realizados. El usuario vuelve al inicio.</t>
@@ -675,22 +735,26 @@
         <v>3.0</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="D5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>26</v>
+      <c r="G5" s="5" t="s">
+        <v>22</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="8" t="s">
-        <v>26</v>
+      <c r="I5" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -716,24 +780,26 @@
         <v>4.0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>28</v>
+      <c r="G6" s="5" t="s">
+        <v>22</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="5" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -759,24 +825,22 @@
         <v>5.0</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="5" t="s">
-        <v>35</v>
+      <c r="I7" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -802,24 +866,24 @@
         <v>6.0</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
@@ -845,24 +909,24 @@
         <v>7.0</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>42</v>
-      </c>
       <c r="D9" s="5" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="5" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
@@ -888,22 +952,24 @@
         <v>8.0</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
-      <c r="F10" s="2"/>
+      <c r="F10" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="5" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
@@ -929,18 +995,20 @@
         <v>9.0</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D11" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="5" t="s">
@@ -973,23 +1041,19 @@
         <v>51</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>56</v>
-      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -1015,24 +1079,22 @@
         <v>11.0</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>60</v>
-      </c>
+      <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="5" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
@@ -1058,24 +1120,26 @@
         <v>12.0</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>62</v>
+      <c r="F14" s="5" t="s">
+        <v>59</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>49</v>
+      <c r="G14" s="9" t="s">
+        <v>60</v>
       </c>
-      <c r="E14" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -1101,22 +1165,24 @@
         <v>13.0</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -1142,18 +1208,20 @@
         <v>14.0</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="F16" s="5"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="5" t="s">
@@ -1183,24 +1251,24 @@
         <v>15.0</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>70</v>
-      </c>
       <c r="D17" s="5" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
@@ -1226,26 +1294,24 @@
         <v>16.0</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>74</v>
+      <c r="C18" s="7" t="s">
+        <v>71</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="G18" s="9" t="s">
-        <v>76</v>
-      </c>
+      <c r="G18" s="2"/>
       <c r="H18" s="2"/>
-      <c r="I18" s="9" t="s">
-        <v>77</v>
+      <c r="I18" s="5" t="s">
+        <v>68</v>
       </c>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
@@ -1267,28 +1333,26 @@
       <c r="AA18" s="2"/>
     </row>
     <row r="19">
-      <c r="A19" s="7">
+      <c r="A19" s="1">
         <v>17.0</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>73</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
-      <c r="F19" s="5" t="s">
-        <v>79</v>
-      </c>
+      <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="5" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
@@ -1310,15 +1374,27 @@
       <c r="AA19" s="2"/>
     </row>
     <row r="20">
-      <c r="A20" s="5"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="A20" s="1">
+        <v>18.0</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F20" s="5"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
+      <c r="I20" s="5" t="s">
+        <v>77</v>
+      </c>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
@@ -1338,16 +1414,30 @@
       <c r="Z20" s="2"/>
       <c r="AA20" s="2"/>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+    <row r="21">
+      <c r="A21" s="1">
+        <v>19.0</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>81</v>
+      </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
+      <c r="I21" s="5" t="s">
+        <v>80</v>
+      </c>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
@@ -1367,16 +1457,32 @@
       <c r="Z21" s="2"/>
       <c r="AA21" s="2"/>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
+    <row r="22">
+      <c r="A22" s="1">
+        <v>20.0</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>85</v>
+      </c>
       <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
+      <c r="I22" s="9" t="s">
+        <v>86</v>
+      </c>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
@@ -1396,16 +1502,30 @@
       <c r="Z22" s="2"/>
       <c r="AA22" s="2"/>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
+    <row r="23">
+      <c r="A23" s="1">
+        <v>21.0</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
+      <c r="I23" s="5" t="s">
+        <v>88</v>
+      </c>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
@@ -1425,8 +1545,8 @@
       <c r="Z23" s="2"/>
       <c r="AA23" s="2"/>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="2"/>
+    <row r="24">
+      <c r="A24" s="5"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -29758,6 +29878,122 @@
       <c r="Z1000" s="2"/>
       <c r="AA1000" s="2"/>
     </row>
+    <row r="1001" ht="15.75" customHeight="1">
+      <c r="A1001" s="2"/>
+      <c r="B1001" s="2"/>
+      <c r="C1001" s="2"/>
+      <c r="D1001" s="2"/>
+      <c r="E1001" s="2"/>
+      <c r="F1001" s="2"/>
+      <c r="G1001" s="2"/>
+      <c r="H1001" s="2"/>
+      <c r="I1001" s="2"/>
+      <c r="J1001" s="2"/>
+      <c r="K1001" s="2"/>
+      <c r="L1001" s="2"/>
+      <c r="M1001" s="2"/>
+      <c r="N1001" s="2"/>
+      <c r="O1001" s="2"/>
+      <c r="P1001" s="2"/>
+      <c r="Q1001" s="2"/>
+      <c r="R1001" s="2"/>
+      <c r="S1001" s="2"/>
+      <c r="T1001" s="2"/>
+      <c r="U1001" s="2"/>
+      <c r="V1001" s="2"/>
+      <c r="W1001" s="2"/>
+      <c r="X1001" s="2"/>
+      <c r="Y1001" s="2"/>
+      <c r="Z1001" s="2"/>
+      <c r="AA1001" s="2"/>
+    </row>
+    <row r="1002" ht="15.75" customHeight="1">
+      <c r="A1002" s="2"/>
+      <c r="B1002" s="2"/>
+      <c r="C1002" s="2"/>
+      <c r="D1002" s="2"/>
+      <c r="E1002" s="2"/>
+      <c r="F1002" s="2"/>
+      <c r="G1002" s="2"/>
+      <c r="H1002" s="2"/>
+      <c r="I1002" s="2"/>
+      <c r="J1002" s="2"/>
+      <c r="K1002" s="2"/>
+      <c r="L1002" s="2"/>
+      <c r="M1002" s="2"/>
+      <c r="N1002" s="2"/>
+      <c r="O1002" s="2"/>
+      <c r="P1002" s="2"/>
+      <c r="Q1002" s="2"/>
+      <c r="R1002" s="2"/>
+      <c r="S1002" s="2"/>
+      <c r="T1002" s="2"/>
+      <c r="U1002" s="2"/>
+      <c r="V1002" s="2"/>
+      <c r="W1002" s="2"/>
+      <c r="X1002" s="2"/>
+      <c r="Y1002" s="2"/>
+      <c r="Z1002" s="2"/>
+      <c r="AA1002" s="2"/>
+    </row>
+    <row r="1003" ht="15.75" customHeight="1">
+      <c r="A1003" s="2"/>
+      <c r="B1003" s="2"/>
+      <c r="C1003" s="2"/>
+      <c r="D1003" s="2"/>
+      <c r="E1003" s="2"/>
+      <c r="F1003" s="2"/>
+      <c r="G1003" s="2"/>
+      <c r="H1003" s="2"/>
+      <c r="I1003" s="2"/>
+      <c r="J1003" s="2"/>
+      <c r="K1003" s="2"/>
+      <c r="L1003" s="2"/>
+      <c r="M1003" s="2"/>
+      <c r="N1003" s="2"/>
+      <c r="O1003" s="2"/>
+      <c r="P1003" s="2"/>
+      <c r="Q1003" s="2"/>
+      <c r="R1003" s="2"/>
+      <c r="S1003" s="2"/>
+      <c r="T1003" s="2"/>
+      <c r="U1003" s="2"/>
+      <c r="V1003" s="2"/>
+      <c r="W1003" s="2"/>
+      <c r="X1003" s="2"/>
+      <c r="Y1003" s="2"/>
+      <c r="Z1003" s="2"/>
+      <c r="AA1003" s="2"/>
+    </row>
+    <row r="1004" ht="15.75" customHeight="1">
+      <c r="A1004" s="2"/>
+      <c r="B1004" s="2"/>
+      <c r="C1004" s="2"/>
+      <c r="D1004" s="2"/>
+      <c r="E1004" s="2"/>
+      <c r="F1004" s="2"/>
+      <c r="G1004" s="2"/>
+      <c r="H1004" s="2"/>
+      <c r="I1004" s="2"/>
+      <c r="J1004" s="2"/>
+      <c r="K1004" s="2"/>
+      <c r="L1004" s="2"/>
+      <c r="M1004" s="2"/>
+      <c r="N1004" s="2"/>
+      <c r="O1004" s="2"/>
+      <c r="P1004" s="2"/>
+      <c r="Q1004" s="2"/>
+      <c r="R1004" s="2"/>
+      <c r="S1004" s="2"/>
+      <c r="T1004" s="2"/>
+      <c r="U1004" s="2"/>
+      <c r="V1004" s="2"/>
+      <c r="W1004" s="2"/>
+      <c r="X1004" s="2"/>
+      <c r="Y1004" s="2"/>
+      <c r="Z1004" s="2"/>
+      <c r="AA1004" s="2"/>
+    </row>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>